<commit_message>
milan sir's name changed to Er. bal Krishna sir in bindhabasini mandir estimate
</commit_message>
<xml_diff>
--- a/ofc/estimates/bindabasini mandir jane sadak dhalaan/बिन्ध्यबासिनी मन्दिर जाने सडक ढलान.xlsx
+++ b/ofc/estimates/bindabasini mandir jane sadak dhalaan/बिन्ध्यबासिनी मन्दिर जाने सडक ढलान.xlsx
@@ -564,6 +564,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -588,22 +606,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -615,18 +627,6 @@
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1266,90 +1266,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="77" t="e">
+      <c r="C6" s="69" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="78"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="10"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -1357,11 +1357,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="9"/>
-      <c r="J6" s="77" t="e">
+      <c r="J6" s="69" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="78"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
@@ -1370,77 +1370,77 @@
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="I7" s="73" t="s">
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="I7" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="71" t="e">
+      <c r="A8" s="77" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="I8" s="74" t="s">
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="I8" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="75" t="e">
+      <c r="A9" s="81" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="I9" s="74" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="I9" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76" t="s">
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="69" t="s">
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="70" t="s">
+      <c r="K11" s="76" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="69"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="12" t="s">
         <v>26</v>
       </c>
@@ -1459,8 +1459,8 @@
       <c r="I12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="69"/>
-      <c r="K12" s="70"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="76"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="e">
@@ -1622,13 +1622,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -1642,6 +1635,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1659,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,113 +1678,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
     </row>
     <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="90" t="s">
+      <c r="A5" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="87" t="s">
+      <c r="H6" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1993,7 +1993,6 @@
         <v>1</v>
       </c>
       <c r="D15" s="40">
-        <f>D10</f>
         <v>14.7</v>
       </c>
       <c r="E15" s="40">
@@ -2468,11 +2467,11 @@
       <c r="B36" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="83">
+      <c r="C36" s="87">
         <f>J34</f>
         <v>226120.14918209484</v>
       </c>
-      <c r="D36" s="83"/>
+      <c r="D36" s="87"/>
       <c r="E36" s="41">
         <v>100</v>
       </c>
@@ -2488,10 +2487,10 @@
       <c r="B37" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="86">
+      <c r="C37" s="90">
         <v>200000</v>
       </c>
-      <c r="D37" s="86"/>
+      <c r="D37" s="90"/>
       <c r="E37" s="41"/>
       <c r="F37" s="51"/>
       <c r="G37" s="50"/>
@@ -2505,11 +2504,11 @@
       <c r="B38" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="86">
+      <c r="C38" s="90">
         <f>C37-C40-C41</f>
         <v>190000</v>
       </c>
-      <c r="D38" s="86"/>
+      <c r="D38" s="90"/>
       <c r="E38" s="41">
         <f>C38/C36*100</f>
         <v>84.026125352939147</v>
@@ -2526,11 +2525,11 @@
       <c r="B39" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="83">
+      <c r="C39" s="87">
         <f>C36-C38</f>
         <v>36120.149182094843</v>
       </c>
-      <c r="D39" s="83"/>
+      <c r="D39" s="87"/>
       <c r="E39" s="41">
         <f>100-E38</f>
         <v>15.973874647060853</v>
@@ -2547,11 +2546,11 @@
       <c r="B40" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="83">
+      <c r="C40" s="87">
         <f>C37*0.03</f>
         <v>6000</v>
       </c>
-      <c r="D40" s="83"/>
+      <c r="D40" s="87"/>
       <c r="E40" s="41">
         <v>3</v>
       </c>
@@ -2567,11 +2566,11 @@
       <c r="B41" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="83">
+      <c r="C41" s="87">
         <f>C37*0.02</f>
         <v>4000</v>
       </c>
-      <c r="D41" s="83"/>
+      <c r="D41" s="87"/>
       <c r="E41" s="41">
         <v>2</v>
       </c>
@@ -2653,13 +2652,6 @@
     <row r="98" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="A7:F7"/>
@@ -2668,13 +2660,20 @@
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LPrepared By:
 Kristal Suwal&amp;CChecked By:
-Er. Milan Phuyal&amp;RApproved By:
+Er. Bal Krishna Manandhar&amp;RApproved By:
 Er. Prakash Singh Saud</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>